<commit_message>
Fixed reporting bugs, added analyse file
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4A7064-32B8-4493-9ABE-35A03F9AC710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5267A6-2228-4D59-9A79-BACB73D9D6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-15300" yWindow="2250" windowWidth="14400" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collective" sheetId="1" r:id="rId1"/>
@@ -893,7 +893,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1073,6 +1073,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1234,9 +1240,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -14364,7 +14371,7 @@
   <dimension ref="A1:N193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14517,47 +14524,47 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>23666158.800000001</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.32400000000000001</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>94.303991999999994</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>94.377994999999999</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>2859630.8</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>4135480.6666669999</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>2287500</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>1567966.6666669999</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <v>280014</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="2">
         <v>36</v>
       </c>
     </row>

</xml_diff>